<commit_message>
Update remaining statistic files for October 2022
</commit_message>
<xml_diff>
--- a/statistics_files/2022/2022.yy.unique borrowers thing.xlsx
+++ b/statistics_files/2022/2022.yy.unique borrowers thing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1704C2AD-621F-49E4-ACE9-E15419DECC40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7461CDFF-426C-4994-903C-E621B5694136}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8670" tabRatio="668" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8670" tabRatio="668" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="91">
   <si>
     <t>branchname</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>2022-09 (September)</t>
+  </si>
+  <si>
+    <t>2022-10 (October)</t>
   </si>
 </sst>
 </file>
@@ -3042,7 +3045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -3104,294 +3107,1067 @@
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="B3" s="3">
+        <v>596</v>
+      </c>
+      <c r="C3" s="3">
+        <v>591</v>
+      </c>
+      <c r="D3" s="3">
+        <v>648</v>
+      </c>
+      <c r="E3" s="3">
+        <v>669</v>
+      </c>
+      <c r="F3" s="3">
+        <v>749</v>
+      </c>
+      <c r="G3" s="3">
+        <v>605</v>
+      </c>
+      <c r="H3" s="3">
+        <v>568</v>
+      </c>
+      <c r="I3" s="3">
+        <v>579</v>
+      </c>
+      <c r="J3" s="3">
+        <v>509</v>
+      </c>
+      <c r="K3" s="3">
+        <v>537</v>
+      </c>
+      <c r="L3" s="3">
+        <v>535</v>
+      </c>
+      <c r="M3" s="3">
+        <v>552</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1850</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
+      <c r="B4">
+        <v>312</v>
+      </c>
+      <c r="C4">
+        <v>331</v>
+      </c>
+      <c r="D4">
+        <v>351</v>
+      </c>
+      <c r="E4">
+        <v>372</v>
+      </c>
+      <c r="F4">
+        <v>409</v>
+      </c>
+      <c r="G4">
+        <v>327</v>
+      </c>
+      <c r="H4">
+        <v>305</v>
+      </c>
+      <c r="I4">
+        <v>313</v>
+      </c>
+      <c r="J4">
+        <v>265</v>
+      </c>
+      <c r="K4">
+        <v>258</v>
+      </c>
+      <c r="L4">
+        <v>254</v>
+      </c>
+      <c r="M4">
+        <v>276</v>
+      </c>
+      <c r="N4">
+        <v>1010</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="B5" s="3">
+        <v>925</v>
+      </c>
+      <c r="C5" s="3">
+        <v>897</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1034</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1072</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1119</v>
+      </c>
+      <c r="G5" s="3">
+        <v>899</v>
+      </c>
+      <c r="H5" s="3">
+        <v>831</v>
+      </c>
+      <c r="I5" s="3">
+        <v>885</v>
+      </c>
+      <c r="J5" s="3">
+        <v>806</v>
+      </c>
+      <c r="K5" s="3">
+        <v>827</v>
+      </c>
+      <c r="L5" s="3">
+        <v>750</v>
+      </c>
+      <c r="M5" s="3">
+        <v>828</v>
+      </c>
+      <c r="N5" s="3">
+        <v>2734</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>29</v>
+      </c>
+      <c r="F6">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>17</v>
+      </c>
+      <c r="H6">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <v>19</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6">
+        <v>15</v>
+      </c>
+      <c r="L6">
+        <v>21</v>
+      </c>
+      <c r="M6">
+        <v>21</v>
+      </c>
+      <c r="N6">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+      <c r="B7" s="3">
+        <v>660</v>
+      </c>
+      <c r="C7" s="3">
+        <v>641</v>
+      </c>
+      <c r="D7" s="3">
+        <v>721</v>
+      </c>
+      <c r="E7" s="3">
+        <v>800</v>
+      </c>
+      <c r="F7" s="3">
+        <v>806</v>
+      </c>
+      <c r="G7" s="3">
+        <v>605</v>
+      </c>
+      <c r="H7" s="3">
+        <v>561</v>
+      </c>
+      <c r="I7" s="3">
+        <v>617</v>
+      </c>
+      <c r="J7" s="3">
+        <v>561</v>
+      </c>
+      <c r="K7" s="3">
+        <v>583</v>
+      </c>
+      <c r="L7" s="3">
+        <v>564</v>
+      </c>
+      <c r="M7" s="3">
+        <v>563</v>
+      </c>
+      <c r="N7" s="3">
+        <v>2187</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
+      <c r="B8">
+        <v>108</v>
+      </c>
+      <c r="C8">
+        <v>108</v>
+      </c>
+      <c r="D8">
+        <v>105</v>
+      </c>
+      <c r="E8">
+        <v>85</v>
+      </c>
+      <c r="F8">
+        <v>79</v>
+      </c>
+      <c r="G8">
+        <v>64</v>
+      </c>
+      <c r="H8">
+        <v>69</v>
+      </c>
+      <c r="I8">
+        <v>73</v>
+      </c>
+      <c r="J8">
+        <v>66</v>
+      </c>
+      <c r="K8">
+        <v>72</v>
+      </c>
+      <c r="L8">
+        <v>78</v>
+      </c>
+      <c r="M8">
+        <v>70</v>
+      </c>
+      <c r="N8">
+        <v>263</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="B9" s="3">
+        <v>109</v>
+      </c>
+      <c r="C9" s="3">
+        <v>112</v>
+      </c>
+      <c r="D9" s="3">
+        <v>123</v>
+      </c>
+      <c r="E9" s="3">
+        <v>120</v>
+      </c>
+      <c r="F9" s="3">
+        <v>126</v>
+      </c>
+      <c r="G9" s="3">
+        <v>108</v>
+      </c>
+      <c r="H9" s="3">
+        <v>103</v>
+      </c>
+      <c r="I9" s="3">
+        <v>124</v>
+      </c>
+      <c r="J9" s="3">
+        <v>93</v>
+      </c>
+      <c r="K9" s="3">
+        <v>104</v>
+      </c>
+      <c r="L9" s="3">
+        <v>99</v>
+      </c>
+      <c r="M9" s="3">
+        <v>99</v>
+      </c>
+      <c r="N9" s="3">
+        <v>377</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
+      <c r="B10">
+        <v>39</v>
+      </c>
+      <c r="C10">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>45</v>
+      </c>
+      <c r="E10">
+        <v>48</v>
+      </c>
+      <c r="F10">
+        <v>67</v>
+      </c>
+      <c r="G10">
+        <v>40</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+      <c r="I10">
+        <v>44</v>
+      </c>
+      <c r="J10">
+        <v>35</v>
+      </c>
+      <c r="K10">
+        <v>33</v>
+      </c>
+      <c r="L10">
+        <v>35</v>
+      </c>
+      <c r="M10">
+        <v>31</v>
+      </c>
+      <c r="N10">
+        <v>106</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3">
+        <v>42</v>
+      </c>
+      <c r="G11" s="3">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3">
+        <v>9</v>
+      </c>
+      <c r="I11" s="3">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3">
+        <v>6</v>
+      </c>
+      <c r="L11" s="3">
+        <v>4</v>
+      </c>
+      <c r="M11" s="3">
+        <v>6</v>
+      </c>
+      <c r="N11" s="3">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="B13" s="3">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3">
+        <v>31</v>
+      </c>
+      <c r="E13" s="3">
+        <v>26</v>
+      </c>
+      <c r="F13" s="3">
+        <v>26</v>
+      </c>
+      <c r="G13" s="3">
+        <v>27</v>
+      </c>
+      <c r="H13" s="3">
+        <v>17</v>
+      </c>
+      <c r="I13" s="3">
+        <v>26</v>
+      </c>
+      <c r="J13" s="3">
+        <v>16</v>
+      </c>
+      <c r="K13" s="3">
+        <v>20</v>
+      </c>
+      <c r="L13" s="3">
+        <v>23</v>
+      </c>
+      <c r="M13" s="3">
+        <v>25</v>
+      </c>
+      <c r="N13" s="3">
+        <v>105</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
+      <c r="B14">
+        <v>54</v>
+      </c>
+      <c r="C14">
+        <v>48</v>
+      </c>
+      <c r="D14">
+        <v>69</v>
+      </c>
+      <c r="E14">
+        <v>62</v>
+      </c>
+      <c r="F14">
+        <v>68</v>
+      </c>
+      <c r="G14">
+        <v>61</v>
+      </c>
+      <c r="H14">
+        <v>50</v>
+      </c>
+      <c r="I14">
+        <v>45</v>
+      </c>
+      <c r="J14">
+        <v>46</v>
+      </c>
+      <c r="K14">
+        <v>41</v>
+      </c>
+      <c r="L14">
+        <v>44</v>
+      </c>
+      <c r="M14">
+        <v>55</v>
+      </c>
+      <c r="N14">
+        <v>180</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="B15" s="3">
+        <v>162</v>
+      </c>
+      <c r="C15" s="3">
+        <v>145</v>
+      </c>
+      <c r="D15" s="3">
+        <v>154</v>
+      </c>
+      <c r="E15" s="3">
+        <v>160</v>
+      </c>
+      <c r="F15" s="3">
+        <v>146</v>
+      </c>
+      <c r="G15" s="3">
+        <v>116</v>
+      </c>
+      <c r="H15" s="3">
+        <v>115</v>
+      </c>
+      <c r="I15" s="3">
+        <v>117</v>
+      </c>
+      <c r="J15" s="3">
+        <v>96</v>
+      </c>
+      <c r="K15" s="3">
+        <v>96</v>
+      </c>
+      <c r="L15" s="3">
+        <v>93</v>
+      </c>
+      <c r="M15" s="3">
+        <v>108</v>
+      </c>
+      <c r="N15" s="3">
+        <v>435</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
+      <c r="B16">
+        <v>62</v>
+      </c>
+      <c r="C16">
+        <v>57</v>
+      </c>
+      <c r="D16">
+        <v>63</v>
+      </c>
+      <c r="E16">
+        <v>66</v>
+      </c>
+      <c r="F16">
+        <v>84</v>
+      </c>
+      <c r="G16">
+        <v>65</v>
+      </c>
+      <c r="H16">
+        <v>65</v>
+      </c>
+      <c r="I16">
+        <v>64</v>
+      </c>
+      <c r="J16">
+        <v>53</v>
+      </c>
+      <c r="K16">
+        <v>63</v>
+      </c>
+      <c r="L16">
+        <v>43</v>
+      </c>
+      <c r="M16">
+        <v>62</v>
+      </c>
+      <c r="N16">
+        <v>211</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="B17" s="3">
+        <v>40</v>
+      </c>
+      <c r="C17" s="3">
+        <v>44</v>
+      </c>
+      <c r="D17" s="3">
+        <v>41</v>
+      </c>
+      <c r="E17" s="3">
+        <v>46</v>
+      </c>
+      <c r="F17" s="3">
+        <v>46</v>
+      </c>
+      <c r="G17" s="3">
+        <v>28</v>
+      </c>
+      <c r="H17" s="3">
+        <v>28</v>
+      </c>
+      <c r="I17" s="3">
+        <v>27</v>
+      </c>
+      <c r="J17" s="3">
+        <v>23</v>
+      </c>
+      <c r="K17" s="3">
+        <v>29</v>
+      </c>
+      <c r="L17" s="3">
+        <v>30</v>
+      </c>
+      <c r="M17" s="3">
+        <v>27</v>
+      </c>
+      <c r="N17" s="3">
+        <v>95</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
+      <c r="B18">
+        <v>215</v>
+      </c>
+      <c r="C18">
+        <v>237</v>
+      </c>
+      <c r="D18">
+        <v>239</v>
+      </c>
+      <c r="E18">
+        <v>257</v>
+      </c>
+      <c r="F18">
+        <v>247</v>
+      </c>
+      <c r="G18">
+        <v>237</v>
+      </c>
+      <c r="H18">
+        <v>183</v>
+      </c>
+      <c r="I18">
+        <v>189</v>
+      </c>
+      <c r="J18">
+        <v>177</v>
+      </c>
+      <c r="K18">
+        <v>186</v>
+      </c>
+      <c r="L18">
+        <v>180</v>
+      </c>
+      <c r="M18">
+        <v>175</v>
+      </c>
+      <c r="N18">
+        <v>644</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="B19" s="3">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3">
+        <v>19</v>
+      </c>
+      <c r="E19" s="3">
+        <v>19</v>
+      </c>
+      <c r="F19" s="3">
+        <v>22</v>
+      </c>
+      <c r="G19" s="3">
+        <v>22</v>
+      </c>
+      <c r="H19" s="3">
+        <v>22</v>
+      </c>
+      <c r="I19" s="3">
+        <v>22</v>
+      </c>
+      <c r="J19" s="3">
+        <v>23</v>
+      </c>
+      <c r="K19" s="3">
+        <v>22</v>
+      </c>
+      <c r="L19" s="3">
+        <v>22</v>
+      </c>
+      <c r="M19" s="3">
+        <v>21</v>
+      </c>
+      <c r="N19" s="3">
+        <v>72</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
+      <c r="B20">
+        <v>310</v>
+      </c>
+      <c r="C20">
+        <v>308</v>
+      </c>
+      <c r="D20">
+        <v>354</v>
+      </c>
+      <c r="E20">
+        <v>359</v>
+      </c>
+      <c r="F20">
+        <v>363</v>
+      </c>
+      <c r="G20">
+        <v>332</v>
+      </c>
+      <c r="H20">
+        <v>297</v>
+      </c>
+      <c r="I20">
+        <v>333</v>
+      </c>
+      <c r="J20">
+        <v>279</v>
+      </c>
+      <c r="K20">
+        <v>274</v>
+      </c>
+      <c r="L20">
+        <v>281</v>
+      </c>
+      <c r="M20">
+        <v>288</v>
+      </c>
+      <c r="N20">
+        <v>950</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
+      <c r="B21" s="3">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3">
+        <v>50</v>
+      </c>
+      <c r="D21" s="3">
+        <v>27</v>
+      </c>
+      <c r="E21" s="3">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3">
+        <v>7</v>
+      </c>
+      <c r="G21" s="3">
+        <v>14</v>
+      </c>
+      <c r="H21" s="3">
+        <v>13</v>
+      </c>
+      <c r="I21" s="3">
+        <v>20</v>
+      </c>
+      <c r="J21" s="3">
+        <v>13</v>
+      </c>
+      <c r="K21" s="3">
+        <v>9</v>
+      </c>
+      <c r="L21" s="3">
+        <v>13</v>
+      </c>
+      <c r="M21" s="3">
+        <v>27</v>
+      </c>
+      <c r="N21" s="3">
+        <v>161</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
+      <c r="B22">
+        <v>366</v>
+      </c>
+      <c r="C22">
+        <v>362</v>
+      </c>
+      <c r="D22">
+        <v>408</v>
+      </c>
+      <c r="E22">
+        <v>364</v>
+      </c>
+      <c r="F22">
+        <v>419</v>
+      </c>
+      <c r="G22">
+        <v>365</v>
+      </c>
+      <c r="H22">
+        <v>354</v>
+      </c>
+      <c r="I22">
+        <v>371</v>
+      </c>
+      <c r="J22">
+        <v>338</v>
+      </c>
+      <c r="K22">
+        <v>353</v>
+      </c>
+      <c r="L22">
+        <v>330</v>
+      </c>
+      <c r="M22">
+        <v>336</v>
+      </c>
+      <c r="N22">
+        <v>1185</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="B23" s="3">
+        <v>32</v>
+      </c>
+      <c r="C23" s="3">
+        <v>28</v>
+      </c>
+      <c r="D23" s="3">
+        <v>54</v>
+      </c>
+      <c r="E23" s="3">
+        <v>43</v>
+      </c>
+      <c r="F23" s="3">
+        <v>39</v>
+      </c>
+      <c r="G23" s="3">
+        <v>26</v>
+      </c>
+      <c r="H23" s="3">
+        <v>22</v>
+      </c>
+      <c r="I23" s="3">
+        <v>23</v>
+      </c>
+      <c r="J23" s="3">
+        <v>28</v>
+      </c>
+      <c r="K23" s="3">
+        <v>24</v>
+      </c>
+      <c r="L23" s="3">
+        <v>27</v>
+      </c>
+      <c r="M23" s="3">
+        <v>37</v>
+      </c>
+      <c r="N23" s="3">
+        <v>177</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
+      <c r="B24">
+        <v>311</v>
+      </c>
+      <c r="C24">
+        <v>370</v>
+      </c>
+      <c r="D24">
+        <v>419</v>
+      </c>
+      <c r="E24">
+        <v>430</v>
+      </c>
+      <c r="F24">
+        <v>443</v>
+      </c>
+      <c r="G24">
+        <v>337</v>
+      </c>
+      <c r="H24">
+        <v>309</v>
+      </c>
+      <c r="I24">
+        <v>321</v>
+      </c>
+      <c r="J24">
+        <v>205</v>
+      </c>
+      <c r="K24">
+        <v>322</v>
+      </c>
+      <c r="L24">
+        <v>281</v>
+      </c>
+      <c r="M24">
+        <v>307</v>
+      </c>
+      <c r="N24">
+        <v>1177</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="B25" s="3">
+        <v>1043</v>
+      </c>
+      <c r="C25" s="3">
+        <v>978</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1181</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1148</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1084</v>
+      </c>
+      <c r="G25" s="3">
+        <v>940</v>
+      </c>
+      <c r="H25" s="3">
+        <v>940</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1015</v>
+      </c>
+      <c r="J25" s="3">
+        <v>888</v>
+      </c>
+      <c r="K25" s="3">
+        <v>842</v>
+      </c>
+      <c r="L25" s="3">
+        <v>904</v>
+      </c>
+      <c r="M25" s="3">
+        <v>930</v>
+      </c>
+      <c r="N25" s="3">
+        <v>3443</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
+      </c>
+      <c r="B26">
+        <v>73</v>
+      </c>
+      <c r="C26">
+        <v>77</v>
+      </c>
+      <c r="D26">
+        <v>78</v>
+      </c>
+      <c r="E26">
+        <v>93</v>
+      </c>
+      <c r="F26">
+        <v>103</v>
+      </c>
+      <c r="G26">
+        <v>97</v>
+      </c>
+      <c r="H26">
+        <v>84</v>
+      </c>
+      <c r="I26">
+        <v>81</v>
+      </c>
+      <c r="J26">
+        <v>66</v>
+      </c>
+      <c r="K26">
+        <v>62</v>
+      </c>
+      <c r="L26">
+        <v>85</v>
+      </c>
+      <c r="M26">
+        <v>95</v>
+      </c>
+      <c r="N26">
+        <v>301</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -3416,327 +4192,1254 @@
       <c r="A28" t="s">
         <v>53</v>
       </c>
+      <c r="B28">
+        <v>111</v>
+      </c>
+      <c r="C28">
+        <v>97</v>
+      </c>
+      <c r="D28">
+        <v>120</v>
+      </c>
+      <c r="E28">
+        <v>114</v>
+      </c>
+      <c r="F28">
+        <v>127</v>
+      </c>
+      <c r="G28">
+        <v>112</v>
+      </c>
+      <c r="H28">
+        <v>104</v>
+      </c>
+      <c r="I28">
+        <v>102</v>
+      </c>
+      <c r="J28">
+        <v>90</v>
+      </c>
+      <c r="K28">
+        <v>94</v>
+      </c>
+      <c r="L28">
+        <v>106</v>
+      </c>
+      <c r="M28">
+        <v>103</v>
+      </c>
+      <c r="N28">
+        <v>322</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
+      <c r="B29" s="3">
+        <v>41</v>
+      </c>
+      <c r="C29" s="3">
+        <v>51</v>
+      </c>
+      <c r="D29" s="3">
+        <v>38</v>
+      </c>
+      <c r="E29" s="3">
+        <v>42</v>
+      </c>
+      <c r="F29" s="3">
+        <v>59</v>
+      </c>
+      <c r="G29" s="3">
+        <v>43</v>
+      </c>
+      <c r="H29" s="3">
+        <v>41</v>
+      </c>
+      <c r="I29" s="3">
+        <v>43</v>
+      </c>
+      <c r="J29" s="3">
+        <v>40</v>
+      </c>
+      <c r="K29" s="3">
+        <v>36</v>
+      </c>
+      <c r="L29" s="3">
+        <v>46</v>
+      </c>
+      <c r="M29" s="3">
+        <v>46</v>
+      </c>
+      <c r="N29" s="3">
+        <v>171</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
+      <c r="B30">
+        <v>182</v>
+      </c>
+      <c r="C30">
+        <v>192</v>
+      </c>
+      <c r="D30">
+        <v>213</v>
+      </c>
+      <c r="E30">
+        <v>222</v>
+      </c>
+      <c r="F30">
+        <v>285</v>
+      </c>
+      <c r="G30">
+        <v>231</v>
+      </c>
+      <c r="H30">
+        <v>192</v>
+      </c>
+      <c r="I30">
+        <v>196</v>
+      </c>
+      <c r="J30">
+        <v>184</v>
+      </c>
+      <c r="K30">
+        <v>192</v>
+      </c>
+      <c r="L30">
+        <v>190</v>
+      </c>
+      <c r="M30">
+        <v>189</v>
+      </c>
+      <c r="N30">
+        <v>559</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
+      <c r="B31" s="3">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3">
+        <v>8</v>
+      </c>
+      <c r="D31" s="3">
+        <v>21</v>
+      </c>
+      <c r="E31" s="3">
+        <v>35</v>
+      </c>
+      <c r="F31" s="3">
+        <v>14</v>
+      </c>
+      <c r="G31" s="3">
+        <v>10</v>
+      </c>
+      <c r="H31" s="3">
+        <v>11</v>
+      </c>
+      <c r="I31" s="3">
+        <v>9</v>
+      </c>
+      <c r="J31" s="3">
+        <v>14</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>17</v>
+      </c>
+      <c r="N31" s="3">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
+      <c r="B32">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>55</v>
+      </c>
+      <c r="E32">
+        <v>54</v>
+      </c>
+      <c r="F32">
+        <v>69</v>
+      </c>
+      <c r="G32">
+        <v>49</v>
+      </c>
+      <c r="H32">
+        <v>34</v>
+      </c>
+      <c r="I32">
+        <v>42</v>
+      </c>
+      <c r="J32">
+        <v>38</v>
+      </c>
+      <c r="K32">
+        <v>31</v>
+      </c>
+      <c r="L32">
+        <v>38</v>
+      </c>
+      <c r="M32">
+        <v>49</v>
+      </c>
+      <c r="N32">
+        <v>155</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
+      <c r="B33" s="3">
+        <v>289</v>
+      </c>
+      <c r="C33" s="3">
+        <v>297</v>
+      </c>
+      <c r="D33" s="3">
+        <v>297</v>
+      </c>
+      <c r="E33" s="3">
+        <v>319</v>
+      </c>
+      <c r="F33" s="3">
+        <v>344</v>
+      </c>
+      <c r="G33" s="3">
+        <v>312</v>
+      </c>
+      <c r="H33" s="3">
+        <v>287</v>
+      </c>
+      <c r="I33" s="3">
+        <v>298</v>
+      </c>
+      <c r="J33" s="3">
+        <v>272</v>
+      </c>
+      <c r="K33" s="3">
+        <v>268</v>
+      </c>
+      <c r="L33" s="3">
+        <v>272</v>
+      </c>
+      <c r="M33" s="3">
+        <v>271</v>
+      </c>
+      <c r="N33" s="3">
+        <v>873</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
+      <c r="B34">
+        <v>210</v>
+      </c>
+      <c r="C34">
+        <v>224</v>
+      </c>
+      <c r="D34">
+        <v>267</v>
+      </c>
+      <c r="E34">
+        <v>258</v>
+      </c>
+      <c r="F34">
+        <v>268</v>
+      </c>
+      <c r="G34">
+        <v>222</v>
+      </c>
+      <c r="H34">
+        <v>239</v>
+      </c>
+      <c r="I34">
+        <v>228</v>
+      </c>
+      <c r="J34">
+        <v>262</v>
+      </c>
+      <c r="K34">
+        <v>291</v>
+      </c>
+      <c r="L34">
+        <v>244</v>
+      </c>
+      <c r="M34">
+        <v>252</v>
+      </c>
+      <c r="N34">
+        <v>793</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="B35" s="3">
+        <v>164</v>
+      </c>
+      <c r="C35" s="3">
+        <v>152</v>
+      </c>
+      <c r="D35" s="3">
+        <v>157</v>
+      </c>
+      <c r="E35" s="3">
+        <v>165</v>
+      </c>
+      <c r="F35" s="3">
+        <v>174</v>
+      </c>
+      <c r="G35" s="3">
+        <v>146</v>
+      </c>
+      <c r="H35" s="3">
+        <v>147</v>
+      </c>
+      <c r="I35" s="3">
+        <v>142</v>
+      </c>
+      <c r="J35" s="3">
+        <v>130</v>
+      </c>
+      <c r="K35" s="3">
+        <v>143</v>
+      </c>
+      <c r="L35" s="3">
+        <v>145</v>
+      </c>
+      <c r="M35" s="3">
+        <v>144</v>
+      </c>
+      <c r="N35" s="3">
+        <v>439</v>
+      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>61</v>
       </c>
+      <c r="B36">
+        <v>779</v>
+      </c>
+      <c r="C36">
+        <v>783</v>
+      </c>
+      <c r="D36">
+        <v>900</v>
+      </c>
+      <c r="E36">
+        <v>943</v>
+      </c>
+      <c r="F36">
+        <v>984</v>
+      </c>
+      <c r="G36">
+        <v>788</v>
+      </c>
+      <c r="H36">
+        <v>665</v>
+      </c>
+      <c r="I36">
+        <v>751</v>
+      </c>
+      <c r="J36">
+        <v>647</v>
+      </c>
+      <c r="K36">
+        <v>640</v>
+      </c>
+      <c r="L36">
+        <v>615</v>
+      </c>
+      <c r="M36">
+        <v>681</v>
+      </c>
+      <c r="N36">
+        <v>2487</v>
+      </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
+      <c r="B37" s="3">
+        <v>146</v>
+      </c>
+      <c r="C37" s="3">
+        <v>153</v>
+      </c>
+      <c r="D37" s="3">
+        <v>165</v>
+      </c>
+      <c r="E37" s="3">
+        <v>180</v>
+      </c>
+      <c r="F37" s="3">
+        <v>181</v>
+      </c>
+      <c r="G37" s="3">
+        <v>155</v>
+      </c>
+      <c r="H37" s="3">
+        <v>136</v>
+      </c>
+      <c r="I37" s="3">
+        <v>150</v>
+      </c>
+      <c r="J37" s="3">
+        <v>144</v>
+      </c>
+      <c r="K37" s="3">
+        <v>139</v>
+      </c>
+      <c r="L37" s="3">
+        <v>139</v>
+      </c>
+      <c r="M37" s="3">
+        <v>129</v>
+      </c>
+      <c r="N37" s="3">
+        <v>426</v>
+      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
+      <c r="B38">
+        <v>480</v>
+      </c>
+      <c r="C38">
+        <v>522</v>
+      </c>
+      <c r="D38">
+        <v>556</v>
+      </c>
+      <c r="E38">
+        <v>609</v>
+      </c>
+      <c r="F38">
+        <v>590</v>
+      </c>
+      <c r="G38">
+        <v>483</v>
+      </c>
+      <c r="H38">
+        <v>403</v>
+      </c>
+      <c r="I38">
+        <v>415</v>
+      </c>
+      <c r="J38">
+        <v>373</v>
+      </c>
+      <c r="K38">
+        <v>383</v>
+      </c>
+      <c r="L38">
+        <v>360</v>
+      </c>
+      <c r="M38">
+        <v>413</v>
+      </c>
+      <c r="N38">
+        <v>1615</v>
+      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
+      <c r="B39" s="3">
+        <v>20</v>
+      </c>
+      <c r="C39" s="3">
+        <v>21</v>
+      </c>
+      <c r="D39" s="3">
+        <v>24</v>
+      </c>
+      <c r="E39" s="3">
+        <v>48</v>
+      </c>
+      <c r="F39" s="3">
+        <v>63</v>
+      </c>
+      <c r="G39" s="3">
+        <v>28</v>
+      </c>
+      <c r="H39" s="3">
+        <v>19</v>
+      </c>
+      <c r="I39" s="3">
+        <v>18</v>
+      </c>
+      <c r="J39" s="3">
+        <v>18</v>
+      </c>
+      <c r="K39" s="3">
+        <v>19</v>
+      </c>
+      <c r="L39" s="3">
+        <v>13</v>
+      </c>
+      <c r="M39" s="3">
+        <v>18</v>
+      </c>
+      <c r="N39" s="3">
+        <v>101</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>65</v>
       </c>
+      <c r="B40">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>26</v>
+      </c>
+      <c r="D40">
+        <v>24</v>
+      </c>
+      <c r="E40">
+        <v>30</v>
+      </c>
+      <c r="F40">
+        <v>32</v>
+      </c>
+      <c r="G40">
+        <v>22</v>
+      </c>
+      <c r="H40">
+        <v>26</v>
+      </c>
+      <c r="I40">
+        <v>37</v>
+      </c>
+      <c r="J40">
+        <v>27</v>
+      </c>
+      <c r="K40">
+        <v>28</v>
+      </c>
+      <c r="L40">
+        <v>24</v>
+      </c>
+      <c r="M40">
+        <v>25</v>
+      </c>
+      <c r="N40">
+        <v>134</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="B41" s="3">
+        <v>122</v>
+      </c>
+      <c r="C41" s="3">
+        <v>114</v>
+      </c>
+      <c r="D41" s="3">
+        <v>140</v>
+      </c>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3">
+        <v>51</v>
+      </c>
+      <c r="H41" s="3">
+        <v>99</v>
+      </c>
+      <c r="I41" s="3">
+        <v>96</v>
+      </c>
+      <c r="J41" s="3">
+        <v>88</v>
+      </c>
+      <c r="K41" s="3">
+        <v>132</v>
+      </c>
+      <c r="L41" s="3">
+        <v>87</v>
+      </c>
+      <c r="M41" s="3">
+        <v>104</v>
+      </c>
+      <c r="N41" s="3">
+        <v>205</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>67</v>
       </c>
+      <c r="B42">
+        <v>363</v>
+      </c>
+      <c r="C42">
+        <v>381</v>
+      </c>
+      <c r="D42">
+        <v>367</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42">
+        <v>328</v>
+      </c>
+      <c r="I42">
+        <v>333</v>
+      </c>
+      <c r="J42">
+        <v>356</v>
+      </c>
+      <c r="K42">
+        <v>362</v>
+      </c>
+      <c r="L42">
+        <v>342</v>
+      </c>
+      <c r="M42">
+        <v>366</v>
+      </c>
+      <c r="N42">
+        <v>503</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="B43" s="3">
+        <v>20</v>
+      </c>
+      <c r="C43" s="3">
+        <v>41</v>
+      </c>
+      <c r="D43" s="3">
+        <v>43</v>
+      </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
+      <c r="G43" s="3">
+        <v>4</v>
+      </c>
+      <c r="H43" s="3">
+        <v>14</v>
+      </c>
+      <c r="I43" s="3">
+        <v>25</v>
+      </c>
+      <c r="J43" s="3">
+        <v>71</v>
+      </c>
+      <c r="K43" s="3">
+        <v>48</v>
+      </c>
+      <c r="L43" s="3">
+        <v>10</v>
+      </c>
+      <c r="M43" s="3">
+        <v>14</v>
+      </c>
+      <c r="N43" s="3">
+        <v>184</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>69</v>
       </c>
+      <c r="B44">
+        <v>99</v>
+      </c>
+      <c r="C44">
+        <v>115</v>
+      </c>
+      <c r="D44">
+        <v>148</v>
+      </c>
+      <c r="G44">
+        <v>19</v>
+      </c>
+      <c r="H44">
+        <v>84</v>
+      </c>
+      <c r="I44">
+        <v>68</v>
+      </c>
+      <c r="J44">
+        <v>59</v>
+      </c>
+      <c r="K44">
+        <v>98</v>
+      </c>
+      <c r="L44">
+        <v>53</v>
+      </c>
+      <c r="M44">
+        <v>117</v>
+      </c>
+      <c r="N44">
+        <v>230</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="B45" s="3">
+        <v>84</v>
+      </c>
+      <c r="C45" s="3">
+        <v>72</v>
+      </c>
+      <c r="D45" s="3">
+        <v>67</v>
+      </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
+      <c r="G45" s="3">
+        <v>8</v>
+      </c>
+      <c r="H45" s="3">
+        <v>86</v>
+      </c>
+      <c r="I45" s="3">
+        <v>86</v>
+      </c>
+      <c r="J45" s="3">
+        <v>93</v>
+      </c>
+      <c r="K45" s="3">
+        <v>89</v>
+      </c>
+      <c r="L45" s="3">
+        <v>70</v>
+      </c>
+      <c r="M45" s="3">
+        <v>73</v>
+      </c>
+      <c r="N45" s="3">
+        <v>149</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>71</v>
       </c>
+      <c r="B46">
+        <v>40</v>
+      </c>
+      <c r="C46">
+        <v>38</v>
+      </c>
+      <c r="D46">
+        <v>40</v>
+      </c>
+      <c r="E46">
+        <v>41</v>
+      </c>
+      <c r="F46">
+        <v>51</v>
+      </c>
+      <c r="G46">
+        <v>40</v>
+      </c>
+      <c r="H46">
+        <v>48</v>
+      </c>
+      <c r="I46">
+        <v>43</v>
+      </c>
+      <c r="J46">
+        <v>40</v>
+      </c>
+      <c r="K46">
+        <v>37</v>
+      </c>
+      <c r="L46">
+        <v>39</v>
+      </c>
+      <c r="M46">
+        <v>33</v>
+      </c>
+      <c r="N46">
+        <v>98</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
+      <c r="B47" s="3">
+        <v>220</v>
+      </c>
+      <c r="C47" s="3">
+        <v>206</v>
+      </c>
+      <c r="D47" s="3">
+        <v>235</v>
+      </c>
+      <c r="E47" s="3">
+        <v>229</v>
+      </c>
+      <c r="F47" s="3">
+        <v>238</v>
+      </c>
+      <c r="G47" s="3">
+        <v>234</v>
+      </c>
+      <c r="H47" s="3">
+        <v>212</v>
+      </c>
+      <c r="I47" s="3">
+        <v>207</v>
+      </c>
+      <c r="J47" s="3">
+        <v>187</v>
+      </c>
+      <c r="K47" s="3">
+        <v>193</v>
+      </c>
+      <c r="L47" s="3">
+        <v>184</v>
+      </c>
+      <c r="M47" s="3">
+        <v>196</v>
+      </c>
+      <c r="N47" s="3">
+        <v>570</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>73</v>
       </c>
+      <c r="B48">
+        <v>280</v>
+      </c>
+      <c r="C48">
+        <v>298</v>
+      </c>
+      <c r="D48">
+        <v>329</v>
+      </c>
+      <c r="E48">
+        <v>309</v>
+      </c>
+      <c r="F48">
+        <v>340</v>
+      </c>
+      <c r="G48">
+        <v>309</v>
+      </c>
+      <c r="H48">
+        <v>274</v>
+      </c>
+      <c r="I48">
+        <v>295</v>
+      </c>
+      <c r="J48">
+        <v>279</v>
+      </c>
+      <c r="K48">
+        <v>271</v>
+      </c>
+      <c r="L48">
+        <v>255</v>
+      </c>
+      <c r="M48">
+        <v>270</v>
+      </c>
+      <c r="N48">
+        <v>782</v>
+      </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
+      <c r="B49" s="3">
+        <v>233</v>
+      </c>
+      <c r="C49" s="3">
+        <v>243</v>
+      </c>
+      <c r="D49" s="3">
+        <v>313</v>
+      </c>
+      <c r="E49" s="3">
+        <v>343</v>
+      </c>
+      <c r="F49" s="3">
+        <v>368</v>
+      </c>
+      <c r="G49" s="3">
+        <v>331</v>
+      </c>
+      <c r="H49" s="3">
+        <v>253</v>
+      </c>
+      <c r="I49" s="3">
+        <v>274</v>
+      </c>
+      <c r="J49" s="3">
+        <v>250</v>
+      </c>
+      <c r="K49" s="3">
+        <v>234</v>
+      </c>
+      <c r="L49" s="3">
+        <v>216</v>
+      </c>
+      <c r="M49" s="3">
+        <v>226</v>
+      </c>
+      <c r="N49" s="3">
+        <v>811</v>
+      </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>75</v>
       </c>
+      <c r="B50">
+        <v>198</v>
+      </c>
+      <c r="C50">
+        <v>212</v>
+      </c>
+      <c r="D50">
+        <v>224</v>
+      </c>
+      <c r="E50">
+        <v>209</v>
+      </c>
+      <c r="F50">
+        <v>212</v>
+      </c>
+      <c r="G50">
+        <v>201</v>
+      </c>
+      <c r="H50">
+        <v>180</v>
+      </c>
+      <c r="I50">
+        <v>181</v>
+      </c>
+      <c r="J50">
+        <v>167</v>
+      </c>
+      <c r="K50">
+        <v>174</v>
+      </c>
+      <c r="L50">
+        <v>171</v>
+      </c>
+      <c r="M50">
+        <v>171</v>
+      </c>
+      <c r="N50">
+        <v>443</v>
+      </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
+      <c r="B51" s="3">
+        <v>500</v>
+      </c>
+      <c r="C51" s="3">
+        <v>499</v>
+      </c>
+      <c r="D51" s="3">
+        <v>595</v>
+      </c>
+      <c r="E51" s="3">
+        <v>628</v>
+      </c>
+      <c r="F51" s="3">
+        <v>645</v>
+      </c>
+      <c r="G51" s="3">
+        <v>556</v>
+      </c>
+      <c r="H51" s="3">
+        <v>472</v>
+      </c>
+      <c r="I51" s="3">
+        <v>486</v>
+      </c>
+      <c r="J51" s="3">
+        <v>406</v>
+      </c>
+      <c r="K51" s="3">
+        <v>409</v>
+      </c>
+      <c r="L51" s="3">
+        <v>407</v>
+      </c>
+      <c r="M51" s="3">
+        <v>419</v>
+      </c>
+      <c r="N51" s="3">
+        <v>1721</v>
+      </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>77</v>
       </c>
+      <c r="B52">
+        <v>73</v>
+      </c>
+      <c r="C52">
+        <v>77</v>
+      </c>
+      <c r="D52">
+        <v>82</v>
+      </c>
+      <c r="E52">
+        <v>74</v>
+      </c>
+      <c r="F52">
+        <v>79</v>
+      </c>
+      <c r="G52">
+        <v>72</v>
+      </c>
+      <c r="H52">
+        <v>70</v>
+      </c>
+      <c r="I52">
+        <v>69</v>
+      </c>
+      <c r="J52">
+        <v>56</v>
+      </c>
+      <c r="K52">
+        <v>63</v>
+      </c>
+      <c r="L52">
+        <v>67</v>
+      </c>
+      <c r="M52">
+        <v>56</v>
+      </c>
+      <c r="N52">
+        <v>233</v>
+      </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
+      <c r="B53" s="3">
+        <v>208</v>
+      </c>
+      <c r="C53" s="3">
+        <v>183</v>
+      </c>
+      <c r="D53" s="3">
+        <v>200</v>
+      </c>
+      <c r="E53" s="3">
+        <v>198</v>
+      </c>
+      <c r="F53" s="3">
+        <v>217</v>
+      </c>
+      <c r="G53" s="3">
+        <v>224</v>
+      </c>
+      <c r="H53" s="3">
+        <v>150</v>
+      </c>
+      <c r="I53" s="3">
+        <v>168</v>
+      </c>
+      <c r="J53" s="3">
+        <v>150</v>
+      </c>
+      <c r="K53" s="3">
+        <v>137</v>
+      </c>
+      <c r="L53" s="3">
+        <v>143</v>
+      </c>
+      <c r="M53" s="3">
+        <v>166</v>
+      </c>
+      <c r="N53" s="3">
+        <v>518</v>
+      </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>79</v>
       </c>
+      <c r="B54">
+        <v>33</v>
+      </c>
+      <c r="C54">
+        <v>35</v>
+      </c>
+      <c r="D54">
+        <v>33</v>
+      </c>
+      <c r="E54">
+        <v>30</v>
+      </c>
+      <c r="F54">
+        <v>42</v>
+      </c>
+      <c r="G54">
+        <v>50</v>
+      </c>
+      <c r="H54">
+        <v>25</v>
+      </c>
+      <c r="I54">
+        <v>31</v>
+      </c>
+      <c r="J54">
+        <v>23</v>
+      </c>
+      <c r="K54">
+        <v>22</v>
+      </c>
+      <c r="L54">
+        <v>28</v>
+      </c>
+      <c r="M54">
+        <v>25</v>
+      </c>
+      <c r="N54">
+        <v>102</v>
+      </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
+      <c r="B55" s="3">
+        <v>35</v>
+      </c>
+      <c r="C55" s="3">
+        <v>37</v>
+      </c>
+      <c r="D55" s="3">
+        <v>42</v>
+      </c>
+      <c r="E55" s="3">
+        <v>43</v>
+      </c>
+      <c r="F55" s="3">
+        <v>49</v>
+      </c>
+      <c r="G55" s="3">
+        <v>33</v>
+      </c>
+      <c r="H55" s="3">
+        <v>38</v>
+      </c>
+      <c r="I55" s="3">
+        <v>38</v>
+      </c>
+      <c r="J55" s="3">
+        <v>26</v>
+      </c>
+      <c r="K55" s="3">
+        <v>30</v>
+      </c>
+      <c r="L55" s="3">
+        <v>29</v>
+      </c>
+      <c r="M55" s="3">
+        <v>31</v>
+      </c>
+      <c r="N55" s="3">
+        <v>143</v>
+      </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>81</v>
+      </c>
+      <c r="B56">
+        <v>50</v>
+      </c>
+      <c r="C56">
+        <v>52</v>
+      </c>
+      <c r="D56">
+        <v>55</v>
+      </c>
+      <c r="E56">
+        <v>62</v>
+      </c>
+      <c r="F56">
+        <v>73</v>
+      </c>
+      <c r="G56">
+        <v>71</v>
+      </c>
+      <c r="H56">
+        <v>63</v>
+      </c>
+      <c r="I56">
+        <v>67</v>
+      </c>
+      <c r="J56">
+        <v>63</v>
+      </c>
+      <c r="K56">
+        <v>65</v>
+      </c>
+      <c r="L56">
+        <v>56</v>
+      </c>
+      <c r="M56">
+        <v>46</v>
+      </c>
+      <c r="N56">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -16893,7 +18596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>